<commit_message>
Final version of accepted paper after reviewing
</commit_message>
<xml_diff>
--- a/figures.xlsx
+++ b/figures.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412852FA-25BA-49F2-B651-1E5AA62A390E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18768" windowHeight="9756" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18768" windowHeight="9756" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="figures_1" sheetId="14" r:id="rId1"/>
     <sheet name="figures_2" sheetId="19" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -414,7 +415,7 @@
                   <a:lumMod val="65000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="38100">
+              <a:ln w="60325">
                 <a:solidFill>
                   <a:srgbClr val="C00000"/>
                 </a:solidFill>
@@ -435,7 +436,7 @@
                     <a:lumMod val="65000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:ln w="38100">
+                <a:ln w="60325">
                   <a:solidFill>
                     <a:srgbClr val="C00000"/>
                   </a:solidFill>
@@ -463,7 +464,7 @@
           </c:dPt>
           <c:trendline>
             <c:spPr>
-              <a:ln w="38100" cap="rnd">
+              <a:ln w="44450" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
@@ -560,7 +561,7 @@
             </c:minus>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -763,7 +764,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -874,7 +875,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -1222,7 +1223,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -1336,7 +1337,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -1722,7 +1723,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -1835,7 +1836,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -2128,7 +2129,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -2236,7 +2237,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -2912,7 +2913,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -3027,7 +3028,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -3197,7 +3198,7 @@
             </c:minus>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3358,11 +3359,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-840000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-1680000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -3385,6 +3386,7 @@
         <c:axId val="620066872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3470,7 +3472,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -3633,7 +3635,7 @@
             </c:minus>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3787,7 +3789,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -3896,7 +3898,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -8941,8 +8943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E752D3-3D99-47F1-9BE2-FE6CACD65DAF}">
   <dimension ref="A1:AN77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C21"/>
+    <sheetView topLeftCell="T13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10315,8 +10317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563198B7-3AFE-4215-811F-D9C6C65CBD82}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>